<commit_message>
El script resuelve calculos vectorizados en vez de utilizar for loops. Los df ahora se guardan en listas, en vez de quedar sueltos en el enviroment
</commit_message>
<xml_diff>
--- a/tp1/cuarta_estimacion.xlsx
+++ b/tp1/cuarta_estimacion.xlsx
@@ -84,563 +84,552 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>313.1010051940947</v>
+        <v>299.9468443580553</v>
       </c>
       <c r="B2" t="n">
-        <v>1.8828182420302344</v>
+        <v>1.9886474699379992</v>
       </c>
       <c r="C2" t="n">
-        <v>-1.0205707631826801</v>
+        <v>-0.9636595695610491</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>299.9468443580553</v>
+        <v>311.14773847666396</v>
       </c>
       <c r="B3" t="n">
-        <v>1.9886474699379992</v>
+        <v>2.0049755339883277</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.9636595695610491</v>
+        <v>-1.1267831787260159</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>314.9250197665565</v>
+        <v>293.5900191095634</v>
       </c>
       <c r="B4" t="n">
-        <v>1.887468839036188</v>
+        <v>2.21276954675977</v>
       </c>
       <c r="C4" t="n">
-        <v>-1.1800383197781301</v>
+        <v>-0.988400062491897</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>297.1174698980124</v>
+        <v>305.4400252289269</v>
       </c>
       <c r="B5" t="n">
-        <v>1.7657724666533703</v>
+        <v>1.902956612567596</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.7987880547195967</v>
+        <v>-1.0405615097602228</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>291.09854555879275</v>
+        <v>302.7973681419485</v>
       </c>
       <c r="B6" t="n">
-        <v>1.9984892611441916</v>
+        <v>1.9350478927000663</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.839598138763102</v>
+        <v>-0.9897465263559363</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>303.700650965937</v>
+        <v>278.79106516956915</v>
       </c>
       <c r="B7" t="n">
-        <v>1.7346217626892675</v>
+        <v>2.265801802008292</v>
       </c>
       <c r="C7" t="n">
-        <v>-0.9575360054727229</v>
+        <v>-0.9295754784372078</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>296.4304785032986</v>
+        <v>314.6212340033373</v>
       </c>
       <c r="B8" t="n">
-        <v>1.8421916992631149</v>
+        <v>1.8928606502430152</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.9056114803187651</v>
+        <v>-1.2104914292014124</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>295.53522825552216</v>
+        <v>288.8306694108422</v>
       </c>
       <c r="B9" t="n">
-        <v>2.0270269595536545</v>
+        <v>1.9930073668326012</v>
       </c>
       <c r="C9" t="n">
-        <v>-1.005249690365148</v>
+        <v>-0.881154869614634</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>301.066060961494</v>
+        <v>293.28128173565705</v>
       </c>
       <c r="B10" t="n">
-        <v>1.9811191871485336</v>
+        <v>2.016476273448693</v>
       </c>
       <c r="C10" t="n">
-        <v>-0.9583768516208291</v>
+        <v>-0.8820076306874003</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>298.99288924825606</v>
+        <v>314.9250197665565</v>
       </c>
       <c r="B11" t="n">
-        <v>2.0799064181379543</v>
+        <v>1.887468839036188</v>
       </c>
       <c r="C11" t="n">
-        <v>-0.9671965434765146</v>
+        <v>-1.1800383197781301</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>289.40986701228513</v>
+        <v>297.1174698980124</v>
       </c>
       <c r="B12" t="n">
-        <v>2.0821628565018333</v>
+        <v>1.7657724666533703</v>
       </c>
       <c r="C12" t="n">
-        <v>-0.9730753862045277</v>
+        <v>-0.7987880547195967</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>295.8612060366306</v>
+        <v>291.09854555879275</v>
       </c>
       <c r="B13" t="n">
-        <v>1.9638773969950263</v>
+        <v>1.9984892611441916</v>
       </c>
       <c r="C13" t="n">
-        <v>-1.0201240474488815</v>
+        <v>-0.839598138763102</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>311.14773847666396</v>
+        <v>303.700650965937</v>
       </c>
       <c r="B14" t="n">
-        <v>2.0049755339883277</v>
+        <v>1.7346217626892675</v>
       </c>
       <c r="C14" t="n">
-        <v>-1.1267831787260159</v>
+        <v>-0.9575360054727229</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>308.14191260070356</v>
+        <v>296.4304785032986</v>
       </c>
       <c r="B15" t="n">
-        <v>1.9502000370830177</v>
+        <v>1.8421916992631149</v>
       </c>
       <c r="C15" t="n">
-        <v>-1.0845055422170364</v>
+        <v>-0.9056114803187651</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>312.36158519753366</v>
+        <v>295.53522825552216</v>
       </c>
       <c r="B16" t="n">
-        <v>1.82896550853489</v>
+        <v>2.0270269595536545</v>
       </c>
       <c r="C16" t="n">
-        <v>-1.0330795358159008</v>
+        <v>-1.005249690365148</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>309.02331515811625</v>
+        <v>301.066060961494</v>
       </c>
       <c r="B17" t="n">
-        <v>1.5039832877679</v>
+        <v>1.9811191871485336</v>
       </c>
       <c r="C17" t="n">
-        <v>-0.8369411233383217</v>
+        <v>-0.9583768516208291</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>301.7003658475296</v>
+        <v>298.99288924825606</v>
       </c>
       <c r="B18" t="n">
-        <v>1.9131902769816842</v>
+        <v>2.0799064181379543</v>
       </c>
       <c r="C18" t="n">
-        <v>-0.9987340104937925</v>
+        <v>-0.9671965434765146</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>306.3086131837516</v>
+        <v>289.40986701228513</v>
       </c>
       <c r="B19" t="n">
-        <v>1.933575172159937</v>
+        <v>2.0821628565018333</v>
       </c>
       <c r="C19" t="n">
-        <v>-1.1207670675435606</v>
+        <v>-0.9730753862045277</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>311.1954306212756</v>
+        <v>295.8612060366306</v>
       </c>
       <c r="B20" t="n">
-        <v>1.829971141213248</v>
+        <v>1.9638773969950263</v>
       </c>
       <c r="C20" t="n">
-        <v>-1.0513841715027088</v>
+        <v>-1.0201240474488815</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>299.72951955610176</v>
+        <v>308.14191260070356</v>
       </c>
       <c r="B21" t="n">
-        <v>1.9264166811862933</v>
+        <v>1.9502000370830177</v>
       </c>
       <c r="C21" t="n">
-        <v>-0.7951797454972417</v>
+        <v>-1.0845055422170364</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>308.0242603359436</v>
+        <v>312.36158519753366</v>
       </c>
       <c r="B22" t="n">
-        <v>1.8484149705322845</v>
+        <v>1.82896550853489</v>
       </c>
       <c r="C22" t="n">
-        <v>-1.061275713332102</v>
+        <v>-1.0330795358159008</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>292.5140104951312</v>
+        <v>309.02331515811625</v>
       </c>
       <c r="B23" t="n">
-        <v>1.8840618460744176</v>
+        <v>1.5039832877679</v>
       </c>
       <c r="C23" t="n">
-        <v>-0.7410037380078798</v>
+        <v>-0.8369411233383217</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>316.50602659791673</v>
+        <v>301.7003658475296</v>
       </c>
       <c r="B24" t="n">
-        <v>1.7444387271296782</v>
+        <v>1.9131902769816842</v>
       </c>
       <c r="C24" t="n">
-        <v>-1.0862605418301323</v>
+        <v>-0.9987340104937925</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>293.5900191095634</v>
+        <v>306.3086131837516</v>
       </c>
       <c r="B25" t="n">
-        <v>2.21276954675977</v>
+        <v>1.933575172159937</v>
       </c>
       <c r="C25" t="n">
-        <v>-0.988400062491897</v>
+        <v>-1.1207670675435606</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>306.0487930540122</v>
+        <v>311.1954306212756</v>
       </c>
       <c r="B26" t="n">
-        <v>1.8798858534006535</v>
+        <v>1.829971141213248</v>
       </c>
       <c r="C26" t="n">
-        <v>-1.0607872934002338</v>
+        <v>-1.0513841715027088</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>281.1177061105754</v>
+        <v>299.72951955610176</v>
       </c>
       <c r="B27" t="n">
-        <v>2.052272695254657</v>
+        <v>1.9264166811862933</v>
       </c>
       <c r="C27" t="n">
-        <v>-0.7048513578789039</v>
+        <v>-0.7951797454972417</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>310.4497019125892</v>
+        <v>308.0242603359436</v>
       </c>
       <c r="B28" t="n">
-        <v>1.9283381295106592</v>
+        <v>1.8484149705322845</v>
       </c>
       <c r="C28" t="n">
-        <v>-1.0443681163572494</v>
+        <v>-1.061275713332102</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>310.84432884340345</v>
+        <v>292.5140104951312</v>
       </c>
       <c r="B29" t="n">
-        <v>1.9604232119222391</v>
+        <v>1.8840618460744176</v>
       </c>
       <c r="C29" t="n">
-        <v>-1.1839624811767226</v>
+        <v>-0.7410037380078798</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>289.91348699104594</v>
+        <v>316.50602659791673</v>
       </c>
       <c r="B30" t="n">
-        <v>2.135380586900032</v>
+        <v>1.7444387271296782</v>
       </c>
       <c r="C30" t="n">
-        <v>-1.0159315718831692</v>
+        <v>-1.0862605418301323</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>291.9735544212472</v>
+        <v>306.0487930540122</v>
       </c>
       <c r="B31" t="n">
-        <v>2.1560368953440032</v>
+        <v>1.8798858534006535</v>
       </c>
       <c r="C31" t="n">
-        <v>-1.011364365655876</v>
+        <v>-1.0607872934002338</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>295.51420590818935</v>
+        <v>281.1177061105754</v>
       </c>
       <c r="B32" t="n">
-        <v>2.1481206961008024</v>
+        <v>2.052272695254657</v>
       </c>
       <c r="C32" t="n">
-        <v>-1.0601778303136262</v>
+        <v>-0.7048513578789039</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>287.65985692220744</v>
+        <v>310.4497019125892</v>
       </c>
       <c r="B33" t="n">
-        <v>2.0760010753148412</v>
+        <v>1.9283381295106592</v>
       </c>
       <c r="C33" t="n">
-        <v>-0.8808939758662092</v>
+        <v>-1.0443681163572494</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>304.79924631630905</v>
+        <v>310.84432884340345</v>
       </c>
       <c r="B34" t="n">
-        <v>1.8160360778679385</v>
+        <v>1.9604232119222391</v>
       </c>
       <c r="C34" t="n">
-        <v>-0.8078139382270659</v>
+        <v>-1.1839624811767226</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>303.6912216786658</v>
+        <v>289.91348699104594</v>
       </c>
       <c r="B35" t="n">
-        <v>2.033844966426333</v>
+        <v>2.135380586900032</v>
       </c>
       <c r="C35" t="n">
-        <v>-1.1259242684460369</v>
+        <v>-1.0159315718831692</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>305.4400252289269</v>
+        <v>291.9735544212472</v>
       </c>
       <c r="B36" t="n">
-        <v>1.902956612567596</v>
+        <v>2.1560368953440032</v>
       </c>
       <c r="C36" t="n">
-        <v>-1.0405615097602228</v>
+        <v>-1.011364365655876</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>298.7671609537739</v>
+        <v>295.51420590818935</v>
       </c>
       <c r="B37" t="n">
-        <v>2.206863718022714</v>
+        <v>2.1481206961008024</v>
       </c>
       <c r="C37" t="n">
-        <v>-1.1194197679033593</v>
+        <v>-1.0601778303136262</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>300.7885664154631</v>
+        <v>287.65985692220744</v>
       </c>
       <c r="B38" t="n">
-        <v>1.8682658018213865</v>
+        <v>2.0760010753148412</v>
       </c>
       <c r="C38" t="n">
-        <v>-0.9077520023487906</v>
+        <v>-0.8808939758662092</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>295.7682577602744</v>
+        <v>304.79924631630905</v>
       </c>
       <c r="B39" t="n">
-        <v>2.044769143187393</v>
+        <v>1.8160360778679385</v>
       </c>
       <c r="C39" t="n">
-        <v>-0.9708087664457066</v>
+        <v>-0.8078139382270659</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>289.57519440403996</v>
+        <v>303.6912216786658</v>
       </c>
       <c r="B40" t="n">
-        <v>2.1824352648702066</v>
+        <v>2.033844966426333</v>
       </c>
       <c r="C40" t="n">
-        <v>-0.9582761577790398</v>
+        <v>-1.1259242684460369</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>296.018820746225</v>
+        <v>298.7671609537739</v>
       </c>
       <c r="B41" t="n">
-        <v>2.056410150646353</v>
+        <v>2.206863718022714</v>
       </c>
       <c r="C41" t="n">
-        <v>-0.9148865468657899</v>
+        <v>-1.1194197679033593</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>292.16458531584686</v>
+        <v>300.7885664154631</v>
       </c>
       <c r="B42" t="n">
-        <v>2.023578355054992</v>
+        <v>1.8682658018213865</v>
       </c>
       <c r="C42" t="n">
-        <v>-1.0284014895437639</v>
+        <v>-0.9077520023487906</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>306.00736653870547</v>
+        <v>295.7682577602744</v>
       </c>
       <c r="B43" t="n">
-        <v>2.051365703630159</v>
+        <v>2.044769143187393</v>
       </c>
       <c r="C43" t="n">
-        <v>-1.213766290622896</v>
+        <v>-0.9708087664457066</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>308.19925715442076</v>
+        <v>289.57519440403996</v>
       </c>
       <c r="B44" t="n">
-        <v>2.034659915275052</v>
+        <v>2.1824352648702066</v>
       </c>
       <c r="C44" t="n">
-        <v>-1.0828098329640194</v>
+        <v>-0.9582761577790398</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>296.90937478287304</v>
+        <v>296.018820746225</v>
       </c>
       <c r="B45" t="n">
-        <v>1.9222067547404746</v>
+        <v>2.056410150646353</v>
       </c>
       <c r="C45" t="n">
-        <v>-0.8530735465760723</v>
+        <v>-0.9148865468657899</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>305.44083406794346</v>
+        <v>292.16458531584686</v>
       </c>
       <c r="B46" t="n">
-        <v>2.0235087111515493</v>
+        <v>2.023578355054992</v>
       </c>
       <c r="C46" t="n">
-        <v>-1.1304663743678722</v>
+        <v>-1.0284014895437639</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>302.7973681419485</v>
+        <v>306.00736653870547</v>
       </c>
       <c r="B47" t="n">
-        <v>1.9350478927000663</v>
+        <v>2.051365703630159</v>
       </c>
       <c r="C47" t="n">
-        <v>-0.9897465263559363</v>
+        <v>-1.213766290622896</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>313.1010051940947</v>
+        <v>308.19925715442076</v>
       </c>
       <c r="B48" t="n">
-        <v>1.8828182420302344</v>
+        <v>2.034659915275052</v>
       </c>
       <c r="C48" t="n">
-        <v>-1.0205707631826801</v>
+        <v>-1.0828098329640194</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>278.79106516956915</v>
+        <v>296.90937478287304</v>
       </c>
       <c r="B49" t="n">
-        <v>2.265801802008292</v>
+        <v>1.9222067547404746</v>
       </c>
       <c r="C49" t="n">
-        <v>-0.9295754784372078</v>
+        <v>-0.8530735465760723</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>314.6212340033373</v>
+        <v>305.44083406794346</v>
       </c>
       <c r="B50" t="n">
-        <v>1.8928606502430152</v>
+        <v>2.0235087111515493</v>
       </c>
       <c r="C50" t="n">
-        <v>-1.2104914292014124</v>
+        <v>-1.1304663743678722</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>288.8306694108422</v>
+        <v>313.1010051940947</v>
       </c>
       <c r="B51" t="n">
-        <v>1.9930073668326012</v>
+        <v>1.8828182420302344</v>
       </c>
       <c r="C51" t="n">
-        <v>-0.881154869614634</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="n">
-        <v>293.28128173565705</v>
-      </c>
-      <c r="B52" t="n">
-        <v>2.016476273448693</v>
-      </c>
-      <c r="C52" t="n">
-        <v>-0.8820076306874003</v>
+        <v>-1.0205707631826801</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
corrijo la generación de dataset para que todas las variables, salvo x2 sean iguales en las dos generaciones de los datos
</commit_message>
<xml_diff>
--- a/tp1/cuarta_estimacion.xlsx
+++ b/tp1/cuarta_estimacion.xlsx
@@ -84,552 +84,552 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>299.9468443580553</v>
+        <v>300.3355232157551</v>
       </c>
       <c r="B2" t="n">
-        <v>1.9886474699379992</v>
+        <v>1.957258766345068</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.9636595695610491</v>
+        <v>-0.992936891014108</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>311.14773847666396</v>
+        <v>302.1200307138862</v>
       </c>
       <c r="B3" t="n">
-        <v>2.0049755339883277</v>
+        <v>1.980089354100932</v>
       </c>
       <c r="C3" t="n">
-        <v>-1.1267831787260159</v>
+        <v>-0.9994303881169618</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>293.5900191095634</v>
+        <v>294.9806523689379</v>
       </c>
       <c r="B4" t="n">
-        <v>2.21276954675977</v>
+        <v>2.1248770935966332</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.988400062491897</v>
+        <v>-1.005548259112435</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>305.4400252289269</v>
+        <v>289.15970945105363</v>
       </c>
       <c r="B5" t="n">
-        <v>1.902956612567596</v>
+        <v>2.059263463833459</v>
       </c>
       <c r="C5" t="n">
-        <v>-1.0405615097602228</v>
+        <v>-0.90551621756431</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>302.7973681419485</v>
+        <v>302.2546139555187</v>
       </c>
       <c r="B6" t="n">
-        <v>1.9350478927000663</v>
+        <v>1.9610693809251658</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.9897465263559363</v>
+        <v>-0.9916869934327884</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>278.79106516956915</v>
+        <v>297.9454685279235</v>
       </c>
       <c r="B7" t="n">
-        <v>2.265801802008292</v>
+        <v>1.8606134021166745</v>
       </c>
       <c r="C7" t="n">
-        <v>-0.9295754784372078</v>
+        <v>-0.8810421064126592</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>314.6212340033373</v>
+        <v>303.1344483809093</v>
       </c>
       <c r="B8" t="n">
-        <v>1.8928606502430152</v>
+        <v>1.9320072656977718</v>
       </c>
       <c r="C8" t="n">
-        <v>-1.2104914292014124</v>
+        <v>-0.8988336229418873</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>288.8306694108422</v>
+        <v>310.29549349639655</v>
       </c>
       <c r="B9" t="n">
-        <v>1.9930073668326012</v>
+        <v>1.9039744372002845</v>
       </c>
       <c r="C9" t="n">
-        <v>-0.881154869614634</v>
+        <v>-1.109354809402632</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>293.28128173565705</v>
+        <v>294.6867198194745</v>
       </c>
       <c r="B10" t="n">
-        <v>2.016476273448693</v>
+        <v>2.0545402293367534</v>
       </c>
       <c r="C10" t="n">
-        <v>-0.8820076306874003</v>
+        <v>-1.053924603653631</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>314.9250197665565</v>
+        <v>292.3151801403916</v>
       </c>
       <c r="B11" t="n">
-        <v>1.887468839036188</v>
+        <v>2.030782533246721</v>
       </c>
       <c r="C11" t="n">
-        <v>-1.1800383197781301</v>
+        <v>-0.9499285749719409</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>297.1174698980124</v>
+        <v>310.92379620920235</v>
       </c>
       <c r="B12" t="n">
-        <v>1.7657724666533703</v>
+        <v>1.9523161365713426</v>
       </c>
       <c r="C12" t="n">
-        <v>-0.7987880547195967</v>
+        <v>-1.080673124955735</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>291.09854555879275</v>
+        <v>292.7880215583621</v>
       </c>
       <c r="B13" t="n">
-        <v>1.9984892611441916</v>
+        <v>1.9769105668579292</v>
       </c>
       <c r="C13" t="n">
-        <v>-0.839598138763102</v>
+        <v>-0.8352055958792949</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>303.700650965937</v>
+        <v>310.96020431255886</v>
       </c>
       <c r="B14" t="n">
-        <v>1.7346217626892675</v>
+        <v>1.8850967138003891</v>
       </c>
       <c r="C14" t="n">
-        <v>-0.9575360054727229</v>
+        <v>-1.0805338955682469</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>296.4304785032986</v>
+        <v>291.8318779832073</v>
       </c>
       <c r="B15" t="n">
-        <v>1.8421916992631149</v>
+        <v>2.168460844260386</v>
       </c>
       <c r="C15" t="n">
-        <v>-0.9056114803187651</v>
+        <v>-1.0157390263736483</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>295.53522825552216</v>
+        <v>299.6280854987036</v>
       </c>
       <c r="B16" t="n">
-        <v>2.0270269595536545</v>
+        <v>1.9675995814451777</v>
       </c>
       <c r="C16" t="n">
-        <v>-1.005249690365148</v>
+        <v>-1.0442245163717248</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>301.066060961494</v>
+        <v>296.03552154118034</v>
       </c>
       <c r="B17" t="n">
-        <v>1.9811191871485336</v>
+        <v>1.9872847762585253</v>
       </c>
       <c r="C17" t="n">
-        <v>-0.9583768516208291</v>
+        <v>-0.8896363166095327</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>298.99288924825606</v>
+        <v>281.4968822759294</v>
       </c>
       <c r="B18" t="n">
-        <v>2.0799064181379543</v>
+        <v>2.262254436321159</v>
       </c>
       <c r="C18" t="n">
-        <v>-0.9671965434765146</v>
+        <v>-0.9670880146686011</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>289.40986701228513</v>
+        <v>289.7510422475379</v>
       </c>
       <c r="B19" t="n">
-        <v>2.0821628565018333</v>
+        <v>2.1320272733355914</v>
       </c>
       <c r="C19" t="n">
-        <v>-0.9730753862045277</v>
+        <v>-0.9176287144317584</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>295.8612060366306</v>
+        <v>300.9899011235117</v>
       </c>
       <c r="B20" t="n">
-        <v>1.9638773969950263</v>
+        <v>2.0407253467456536</v>
       </c>
       <c r="C20" t="n">
-        <v>-1.0201240474488815</v>
+        <v>-0.9470525681715379</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>308.14191260070356</v>
+        <v>314.5510878791318</v>
       </c>
       <c r="B21" t="n">
-        <v>1.9502000370830177</v>
+        <v>1.8368188990294851</v>
       </c>
       <c r="C21" t="n">
-        <v>-1.0845055422170364</v>
+        <v>-1.0612728776735716</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>312.36158519753366</v>
+        <v>309.37266044769</v>
       </c>
       <c r="B22" t="n">
-        <v>1.82896550853489</v>
+        <v>1.962303121056252</v>
       </c>
       <c r="C22" t="n">
-        <v>-1.0330795358159008</v>
+        <v>-1.2230256489273788</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>309.02331515811625</v>
+        <v>290.8685550266593</v>
       </c>
       <c r="B23" t="n">
-        <v>1.5039832877679</v>
+        <v>1.7328592134996328</v>
       </c>
       <c r="C23" t="n">
-        <v>-0.8369411233383217</v>
+        <v>-0.7415550546033299</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>301.7003658475296</v>
+        <v>307.4661665965745</v>
       </c>
       <c r="B24" t="n">
-        <v>1.9131902769816842</v>
+        <v>1.8916815140183176</v>
       </c>
       <c r="C24" t="n">
-        <v>-0.9987340104937925</v>
+        <v>-1.0464894413129464</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>306.3086131837516</v>
+        <v>286.130226637444</v>
       </c>
       <c r="B25" t="n">
-        <v>1.933575172159937</v>
+        <v>2.053339628956805</v>
       </c>
       <c r="C25" t="n">
-        <v>-1.1207670675435606</v>
+        <v>-0.847251885582815</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>311.1954306212756</v>
+        <v>291.56081428278924</v>
       </c>
       <c r="B26" t="n">
-        <v>1.829971141213248</v>
+        <v>2.1026098217250664</v>
       </c>
       <c r="C26" t="n">
-        <v>-1.0513841715027088</v>
+        <v>-0.9187012329173585</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>299.72951955610176</v>
+        <v>280.74453440569374</v>
       </c>
       <c r="B27" t="n">
-        <v>1.9264166811862933</v>
+        <v>2.142512501556268</v>
       </c>
       <c r="C27" t="n">
-        <v>-0.7951797454972417</v>
+        <v>-0.7445160704077327</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>308.0242603359436</v>
+        <v>298.5983602861604</v>
       </c>
       <c r="B28" t="n">
-        <v>1.8484149705322845</v>
+        <v>2.067537883277829</v>
       </c>
       <c r="C28" t="n">
-        <v>-1.061275713332102</v>
+        <v>-0.949949721865206</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>292.5140104951312</v>
+        <v>306.4441611523221</v>
       </c>
       <c r="B29" t="n">
-        <v>1.8840618460744176</v>
+        <v>1.997686802816628</v>
       </c>
       <c r="C29" t="n">
-        <v>-0.7410037380078798</v>
+        <v>-1.2795351469796803</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>316.50602659791673</v>
+        <v>313.6710454585673</v>
       </c>
       <c r="B30" t="n">
-        <v>1.7444387271296782</v>
+        <v>1.8970643097674358</v>
       </c>
       <c r="C30" t="n">
-        <v>-1.0862605418301323</v>
+        <v>-1.1744243833540473</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>306.0487930540122</v>
+        <v>306.4257822135574</v>
       </c>
       <c r="B31" t="n">
-        <v>1.8798858534006535</v>
+        <v>1.6451993185596387</v>
       </c>
       <c r="C31" t="n">
-        <v>-1.0607872934002338</v>
+        <v>-1.061695474348634</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>281.1177061105754</v>
+        <v>306.77379100771645</v>
       </c>
       <c r="B32" t="n">
-        <v>2.052272695254657</v>
+        <v>1.8504152560696963</v>
       </c>
       <c r="C32" t="n">
-        <v>-0.7048513578789039</v>
+        <v>-0.9517126569887219</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>310.4497019125892</v>
+        <v>299.308409746554</v>
       </c>
       <c r="B33" t="n">
-        <v>1.9283381295106592</v>
+        <v>1.8690669403358098</v>
       </c>
       <c r="C33" t="n">
-        <v>-1.0443681163572494</v>
+        <v>-0.8700582158107949</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>310.84432884340345</v>
+        <v>284.8599381559061</v>
       </c>
       <c r="B34" t="n">
-        <v>1.9604232119222391</v>
+        <v>2.0868168454552887</v>
       </c>
       <c r="C34" t="n">
-        <v>-1.1839624811767226</v>
+        <v>-0.6939105074909117</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>289.91348699104594</v>
+        <v>289.61163173933676</v>
       </c>
       <c r="B35" t="n">
-        <v>2.135380586900032</v>
+        <v>2.202873862545679</v>
       </c>
       <c r="C35" t="n">
-        <v>-1.0159315718831692</v>
+        <v>-0.9017881676650067</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>291.9735544212472</v>
+        <v>317.39431312219824</v>
       </c>
       <c r="B36" t="n">
-        <v>2.1560368953440032</v>
+        <v>2.0550300801755474</v>
       </c>
       <c r="C36" t="n">
-        <v>-1.011364365655876</v>
+        <v>-1.18847985427789</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>295.51420590818935</v>
+        <v>300.7989692939087</v>
       </c>
       <c r="B37" t="n">
-        <v>2.1481206961008024</v>
+        <v>1.9462252028006335</v>
       </c>
       <c r="C37" t="n">
-        <v>-1.0601778303136262</v>
+        <v>-0.8341201110147657</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>287.65985692220744</v>
+        <v>298.3239323386273</v>
       </c>
       <c r="B38" t="n">
-        <v>2.0760010753148412</v>
+        <v>2.031401409946047</v>
       </c>
       <c r="C38" t="n">
-        <v>-0.8808939758662092</v>
+        <v>-0.9036463576448129</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>304.79924631630905</v>
+        <v>302.71891016388304</v>
       </c>
       <c r="B39" t="n">
-        <v>1.8160360778679385</v>
+        <v>1.9644733930312515</v>
       </c>
       <c r="C39" t="n">
-        <v>-0.8078139382270659</v>
+        <v>-1.0951252678531198</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>303.6912216786658</v>
+        <v>283.1878730597422</v>
       </c>
       <c r="B40" t="n">
-        <v>2.033844966426333</v>
+        <v>2.0876519191470213</v>
       </c>
       <c r="C40" t="n">
-        <v>-1.1259242684460369</v>
+        <v>-0.8811489338448948</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>298.7671609537739</v>
+        <v>311.87880288575917</v>
       </c>
       <c r="B41" t="n">
-        <v>2.206863718022714</v>
+        <v>1.806598127398824</v>
       </c>
       <c r="C41" t="n">
-        <v>-1.1194197679033593</v>
+        <v>-1.0793389056618605</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>300.7885664154631</v>
+        <v>302.9565813451401</v>
       </c>
       <c r="B42" t="n">
-        <v>1.8682658018213865</v>
+        <v>1.993150432715906</v>
       </c>
       <c r="C42" t="n">
-        <v>-0.9077520023487906</v>
+        <v>-1.0531365733667242</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>295.7682577602744</v>
+        <v>296.1524203127572</v>
       </c>
       <c r="B43" t="n">
-        <v>2.044769143187393</v>
+        <v>1.959602768288211</v>
       </c>
       <c r="C43" t="n">
-        <v>-0.9708087664457066</v>
+        <v>-0.95255380053481</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>289.57519440403996</v>
+        <v>304.1785610371654</v>
       </c>
       <c r="B44" t="n">
-        <v>2.1824352648702066</v>
+        <v>2.0147758924845425</v>
       </c>
       <c r="C44" t="n">
-        <v>-0.9582761577790398</v>
+        <v>-1.02093745746713</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>296.018820746225</v>
+        <v>299.3055371877944</v>
       </c>
       <c r="B45" t="n">
-        <v>2.056410150646353</v>
+        <v>2.028598707105818</v>
       </c>
       <c r="C45" t="n">
-        <v>-0.9148865468657899</v>
+        <v>-1.052427054073405</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>292.16458531584686</v>
+        <v>306.8767724289121</v>
       </c>
       <c r="B46" t="n">
-        <v>2.023578355054992</v>
+        <v>1.8562698350065303</v>
       </c>
       <c r="C46" t="n">
-        <v>-1.0284014895437639</v>
+        <v>-1.0336616931180485</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>306.00736653870547</v>
+        <v>313.4969054504496</v>
       </c>
       <c r="B47" t="n">
-        <v>2.051365703630159</v>
+        <v>1.9906804906896645</v>
       </c>
       <c r="C47" t="n">
-        <v>-1.213766290622896</v>
+        <v>-1.1516786159257915</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>308.19925715442076</v>
+        <v>327.1735481510344</v>
       </c>
       <c r="B48" t="n">
-        <v>2.034659915275052</v>
+        <v>1.8260559478626412</v>
       </c>
       <c r="C48" t="n">
-        <v>-1.0828098329640194</v>
+        <v>-1.1976155147061642</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>296.90937478287304</v>
+        <v>291.7469532430533</v>
       </c>
       <c r="B49" t="n">
-        <v>1.9222067547404746</v>
+        <v>2.326455427492738</v>
       </c>
       <c r="C49" t="n">
-        <v>-0.8530735465760723</v>
+        <v>-1.1265704347145413</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>305.44083406794346</v>
+        <v>299.3478342051676</v>
       </c>
       <c r="B50" t="n">
-        <v>2.0235087111515493</v>
+        <v>2.1513291173058073</v>
       </c>
       <c r="C50" t="n">
-        <v>-1.1304663743678722</v>
+        <v>-1.1291722852937272</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>313.1010051940947</v>
+        <v>282.72988090050416</v>
       </c>
       <c r="B51" t="n">
-        <v>1.8828182420302344</v>
+        <v>2.0256078860126054</v>
       </c>
       <c r="C51" t="n">
-        <v>-1.0205707631826801</v>
+        <v>-0.7394940549859654</v>
       </c>
     </row>
   </sheetData>

</xml_diff>